<commit_message>
add one more scenario in datatable test
</commit_message>
<xml_diff>
--- a/src/test/resources/excel.xlsx
+++ b/src/test/resources/excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\eclipse-workspace\excelbdd-test\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B4856E-ADA9-43C7-A5F0-8CC9C9E281CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF545CB-08AB-4978-A8F2-7963A6EBFA75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FirstSheet" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="55">
   <si>
     <t>Feature: Is it Friday yet?</t>
   </si>
@@ -199,18 +199,29 @@
   </si>
   <si>
     <t>pass</t>
+  </si>
+  <si>
+    <t>Monday</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -452,75 +463,77 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -807,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FB6D792-3148-423C-85CF-2B9A701A4234}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -987,10 +1000,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA61B7C-E7D5-44B9-B67D-3CDC93FF04F4}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1003,7 +1016,7 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="8" t="s">
         <v>15</v>
       </c>
@@ -1011,19 +1024,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1039,8 +1052,11 @@
       <c r="E4" s="7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="35" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1056,8 +1072,11 @@
       <c r="E5" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="30">
+      <c r="F5" s="36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30">
       <c r="A6" s="6" t="s">
         <v>9</v>
       </c>
@@ -1073,8 +1092,11 @@
       <c r="E6" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1088,6 +1110,9 @@
         <v>18</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add WeekManager and its test
</commit_message>
<xml_diff>
--- a/src/test/resources/excel.xlsx
+++ b/src/test/resources/excel.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\eclipse-workspace\excelbdd-test\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF545CB-08AB-4978-A8F2-7963A6EBFA75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6456FF-D54C-45AB-ACD0-A7D966C66FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FirstSheet" sheetId="3" r:id="rId1"/>
-    <sheet name="WeekDayCheck" sheetId="2" r:id="rId2"/>
-    <sheet name="Expected1" sheetId="4" r:id="rId3"/>
-    <sheet name="TestResult1" sheetId="5" r:id="rId4"/>
+    <sheet name="FridayCheck" sheetId="6" r:id="rId2"/>
+    <sheet name="WeekDayCheck" sheetId="2" r:id="rId3"/>
+    <sheet name="Expected1" sheetId="4" r:id="rId4"/>
+    <sheet name="TestResult1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="57">
   <si>
     <t>Feature: Is it Friday yet?</t>
   </si>
@@ -202,18 +203,32 @@
   </si>
   <si>
     <t>Monday</t>
+  </si>
+  <si>
+    <t>TGIF</t>
+  </si>
+  <si>
+    <t>When I ask whether it's Friday yet？Then I should be told</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -463,77 +478,81 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -931,7 +950,7 @@
       <c r="G6" s="16"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="27" t="s">
         <v>38</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -944,7 +963,7 @@
       <c r="G7" s="16"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="26"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="10" t="s">
         <v>40</v>
       </c>
@@ -955,7 +974,7 @@
       <c r="G8" s="16"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="29" t="s">
         <v>41</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -978,7 +997,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="28"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="20" t="s">
         <v>40</v>
       </c>
@@ -999,11 +1018,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA61B7C-E7D5-44B9-B67D-3CDC93FF04F4}">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54BB8987-3CB4-49AF-9611-E701C12ED542}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1025,11 +1044,11 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
     </row>
     <row r="3" spans="1:6">
       <c r="B3" s="1" t="s">
@@ -1052,7 +1071,7 @@
       <c r="E4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="25" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1072,7 +1091,117 @@
       <c r="E5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="45">
+      <c r="A6" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{5EE1B2C9-8D37-437F-B0EC-45CAA9A4A4E3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA61B7C-E7D5-44B9-B67D-3CDC93FF04F4}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="26" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1128,7 +1257,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABA8FF02-C753-4950-8E4D-F90C1C2043E8}">
   <dimension ref="A1:L11"/>
   <sheetViews>
@@ -1149,24 +1278,24 @@
       <c r="B1" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="30" t="s">
+      <c r="D1" s="33"/>
+      <c r="E1" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="30" t="s">
+      <c r="F1" s="33"/>
+      <c r="G1" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="32" t="s">
+      <c r="H1" s="33"/>
+      <c r="I1" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="33"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="31"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="33"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="10" t="s">
@@ -1367,12 +1496,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C77002CD-FBD5-4D6F-A13A-35D9AB6E7D64}">
   <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:Z1048576"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1397,31 +1526,31 @@
       <c r="B1" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="30" t="s">
+      <c r="D1" s="33"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="34"/>
-      <c r="R1" s="30" t="s">
+      <c r="G1" s="33"/>
+      <c r="H1" s="36"/>
+      <c r="R1" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="S1" s="31"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="32" t="s">
+      <c r="S1" s="33"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="30" t="s">
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="34"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="36"/>
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="10" t="s">

</xml_diff>